<commit_message>
fixed #10, #9, #8
</commit_message>
<xml_diff>
--- a/Flashcards.xlsx
+++ b/Flashcards.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfitz\Google Drive\Docs\VSCode\Anki\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Documents\GitHub Clones\anki-card-importer-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F87AB7-7969-4C81-8829-756B88FEEC60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EAFBBA-77A3-4DB5-B34C-66BCC5EFC897}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15465" yWindow="1785" windowWidth="11775" windowHeight="12375" tabRatio="803" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19515" yWindow="6630" windowWidth="18570" windowHeight="17640" tabRatio="777" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="(Test) Korean {Large}" sheetId="11" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="180">
   <si>
     <t>FOREIGN</t>
   </si>
@@ -507,17 +507,6 @@
   </si>
   <si>
     <t>고령</t>
-  </si>
-  <si>
-    <t>비밀</t>
-  </si>
-  <si>
-    <t>1.
-secret
-2.
-confidential
-3.
-classified</t>
   </si>
   <si>
     <t>1.
@@ -528,31 +517,10 @@
 elderly</t>
   </si>
   <si>
-    <t>번호</t>
-  </si>
-  <si>
-    <t>전화</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>phone call, (telephone) call; (전화기) telephone, phone, call (up), phone, (Brit) ring</t>
-  </si>
-  <si>
-    <t>教师</t>
-  </si>
-  <si>
     <t>中文</t>
   </si>
   <si>
     <t>日本語</t>
-  </si>
-  <si>
-    <t>1n. teacher</t>
-  </si>
-  <si>
-    <t>1n.shark</t>
   </si>
   <si>
     <t>1n. elephant</t>
@@ -628,6 +596,12 @@
   </si>
   <si>
     <t>1n. fool</t>
+  </si>
+  <si>
+    <t>전화</t>
+  </si>
+  <si>
+    <t>바보</t>
   </si>
 </sst>
 </file>
@@ -644,22 +618,26 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="16"/>
@@ -670,6 +648,7 @@
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1018,7 +997,7 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -5160,10 +5139,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFBE6AD-A12D-4329-A39D-5AB8422E3BA3}">
-  <dimension ref="A1:Z992"/>
+  <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -5225,49 +5204,40 @@
         <v>151</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C3" s="15"/>
     </row>
-    <row r="4" spans="1:26" ht="120">
-      <c r="A4" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="C4" s="15"/>
+    <row r="4" spans="1:26">
+      <c r="A4" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>157</v>
+      <c r="A5" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:26" ht="45">
-      <c r="A6" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>158</v>
-      </c>
+    <row r="6" spans="1:26">
+      <c r="A6" s="1"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="4"/>
-      <c r="B7" s="17"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="4"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" s="1"/>
-      <c r="B9" s="22"/>
       <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:26">
@@ -5277,30 +5247,31 @@
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="1"/>
-      <c r="B11" s="22"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:26">
-      <c r="A12" s="1"/>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A12" s="4"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:26">
-      <c r="A13" s="1"/>
-      <c r="B13" s="22"/>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A13" s="4"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:26">
-      <c r="A14" s="1"/>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A14" s="4"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="22"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A16" s="4"/>
-      <c r="B16" s="23"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1">
@@ -5314,8 +5285,8 @@
       <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A19" s="15"/>
-      <c r="B19" s="19"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
@@ -5325,7 +5296,7 @@
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="A21" s="4"/>
-      <c r="B21" s="19"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="4"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
@@ -5335,22 +5306,19 @@
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="A23" s="4"/>
-      <c r="B23" s="19"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
       <c r="A24" s="4"/>
-      <c r="B24" s="23"/>
       <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1">
       <c r="A25" s="4"/>
-      <c r="B25" s="23"/>
       <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="4"/>
-      <c r="B26" s="23"/>
       <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
@@ -9204,18 +9172,6 @@
     <row r="989" spans="1:3" ht="15.75" customHeight="1">
       <c r="A989" s="4"/>
       <c r="C989" s="4"/>
-    </row>
-    <row r="990" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A990" s="4"/>
-      <c r="C990" s="4"/>
-    </row>
-    <row r="991" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A991" s="4"/>
-      <c r="C991" s="4"/>
-    </row>
-    <row r="992" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A992" s="4"/>
-      <c r="C992" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -9232,8 +9188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -9262,7 +9218,7 @@
         <v>145</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -9286,7 +9242,7 @@
         <v>57</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1">
@@ -9294,7 +9250,7 @@
         <v>58</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -9302,7 +9258,7 @@
         <v>125</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -9312,7 +9268,7 @@
         <v>126</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -9323,7 +9279,7 @@
         <v>127</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -9334,7 +9290,7 @@
         <v>128</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -9345,7 +9301,7 @@
         <v>129</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -9356,7 +9312,7 @@
         <v>130</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -9367,7 +9323,7 @@
         <v>131</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -9378,7 +9334,7 @@
         <v>132</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -9389,7 +9345,7 @@
         <v>133</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -9400,7 +9356,7 @@
         <v>134</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -9411,7 +9367,7 @@
         <v>135</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -9422,7 +9378,7 @@
         <v>136</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -9433,7 +9389,7 @@
         <v>137</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -9444,7 +9400,7 @@
         <v>138</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -9455,7 +9411,7 @@
         <v>139</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -9466,7 +9422,7 @@
         <v>140</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -9477,7 +9433,7 @@
         <v>141</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -9496,10 +9452,10 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1">
       <c r="A25" s="26" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -9510,7 +9466,7 @@
         <v>143</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C26" s="6"/>
     </row>
@@ -9519,7 +9475,7 @@
         <v>144</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1"/>
@@ -10508,10 +10464,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E33525-EC00-4AF9-951F-E9727E4AC919}">
-  <dimension ref="A1:E998"/>
+  <dimension ref="A1:E995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -10540,40 +10496,37 @@
         <v>145</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30">
       <c r="A3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>163</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>147</v>
-      </c>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>148</v>
-      </c>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -10641,23 +10594,23 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -10678,33 +10631,15 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="6"/>
-      <c r="B21" s="25"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
-      <c r="B25" s="24"/>
-    </row>
+      <c r="B22" s="24"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="26" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="27" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="28" spans="1:5" ht="15.75" customHeight="1"/>
@@ -11675,9 +11610,6 @@
     <row r="993" ht="15.75" customHeight="1"/>
     <row r="994" ht="15.75" customHeight="1"/>
     <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2" xr:uid="{7FB997AC-A231-4A4A-A6D1-6C6A3F7C34B9}">
@@ -11724,7 +11656,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:5">

</xml_diff>